<commit_message>
Successfully mongoDB integration for HTML page code pushed
</commit_message>
<xml_diff>
--- a/datalist.xlsx
+++ b/datalist.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d955012\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB9ED30-8024-4E8D-ABB5-B4CC239CFD73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4CC67B58-98EA-47C2-9163-8D77A827F324}"/>
+    <workbookView xWindow="0" yWindow="2448" windowWidth="16980" windowHeight="8232"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -60,9 +55,6 @@
     <t>Ranjan</t>
   </si>
   <si>
-    <t>nityaranjan1906453@gmail.com</t>
-  </si>
-  <si>
     <t>Atmosol</t>
   </si>
   <si>
@@ -72,19 +64,22 @@
     <t>Kumar</t>
   </si>
   <si>
-    <t>abhay4563@gmail.com</t>
-  </si>
-  <si>
     <t>7303709376</t>
   </si>
   <si>
     <t>3234556754</t>
+  </si>
+  <si>
+    <t>abhay43@gmail.com</t>
+  </si>
+  <si>
+    <t>nityaranjan163@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -188,7 +183,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -240,7 +235,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -434,31 +429,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD3C6E3E-2E71-4662-921B-DB835830D78E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -478,7 +473,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -486,42 +481,42 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{64A8F315-238A-4A43-BB0C-56A1DFFC1CFD}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{66823179-EE4B-4C09-ACA1-BE2EEC074B10}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
New code pushed by HP
</commit_message>
<xml_diff>
--- a/datalist.xlsx
+++ b/datalist.xlsx
@@ -70,10 +70,10 @@
     <t>3234556754</t>
   </si>
   <si>
-    <t>abhay43@gmail.com</t>
-  </si>
-  <si>
-    <t>nityaranjan163@gmail.com</t>
+    <t>nityaranjn7897756843@gmail.com</t>
+  </si>
+  <si>
+    <t>abh090653646@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -429,7 +429,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -440,14 +440,14 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
@@ -481,7 +481,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>11</v>
@@ -501,7 +501,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Sauce labs integration code pushed for Grid
</commit_message>
<xml_diff>
--- a/datalist.xlsx
+++ b/datalist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2448" windowWidth="16980" windowHeight="8232"/>
+    <workbookView xWindow="0" yWindow="2448" windowWidth="12864" windowHeight="5448"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -70,10 +70,10 @@
     <t>3234556754</t>
   </si>
   <si>
-    <t>nityaranjn7897756843@gmail.com</t>
-  </si>
-  <si>
-    <t>abh090653646@gmail.com</t>
+    <t>abh0906536897454546@gmail.com</t>
+  </si>
+  <si>
+    <t>nityaranjn78977344643@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -429,7 +429,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -440,14 +440,14 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
@@ -481,7 +481,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>11</v>
@@ -501,7 +501,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
working code for saucelab is pushed
</commit_message>
<xml_diff>
--- a/datalist.xlsx
+++ b/datalist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2448" windowWidth="12864" windowHeight="5448"/>
+    <workbookView xWindow="0" yWindow="2448" windowWidth="16980" windowHeight="8232"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -70,10 +70,10 @@
     <t>3234556754</t>
   </si>
   <si>
-    <t>nityaranjn7897344643@gmail.com</t>
-  </si>
-  <si>
-    <t>abh090653687454546@gmail.com</t>
+    <t>nityaranjn55623@gmail.com</t>
+  </si>
+  <si>
+    <t>abh09082444@gmail.com</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
BrowserStack Integration Code is pushed
</commit_message>
<xml_diff>
--- a/datalist.xlsx
+++ b/datalist.xlsx
@@ -70,10 +70,10 @@
     <t>3234556754</t>
   </si>
   <si>
-    <t>nityaranjn55623@gmail.com</t>
-  </si>
-  <si>
-    <t>abh09082444@gmail.com</t>
+    <t>nityaranjn623@gmail.com</t>
+  </si>
+  <si>
+    <t>abh090824@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -429,7 +429,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -440,7 +440,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>